<commit_message>
feat：update lightdragon 1 and 4
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
+++ b/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -79,13 +79,22 @@
     <t xml:space="preserve">10|10|100</t>
   </si>
   <si>
-    <t xml:space="preserve">E141AC6246FA01BC41E98BB4D9423F80E141AC6246FA01BC41E98BB4D9423F80</t>
+    <t xml:space="preserve">E141AC6246FA01BC41E98BB4D9423F80</t>
   </si>
   <si>
-    <t xml:space="preserve">0|0|150</t>
+    <t xml:space="preserve">0|0|100</t>
   </si>
   <si>
-    <t xml:space="preserve">E0D79BB64C2DCD08AEC54388C11A6AE7E0D79BB64C2DCD08AEC54388C11A6AE7</t>
+    <t xml:space="preserve">E0D79BB64C2DCD08AEC54388C11A6AE7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1D729A16497C24D2C4B6A9A247F09AE9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C030E576410EBE92DF5FAB83FAFD859A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-60|0|70</t>
   </si>
 </sst>
 </file>
@@ -477,7 +486,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topRight" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,10 +693,22 @@
       <c r="ALU7" s="8"/>
     </row>
     <row r="8" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>23</v>
+      </c>
       <c r="D8" s="13"/>
+      <c r="E8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G8" s="11"/>
       <c r="I8" s="11"/>
       <c r="ALS8" s="8"/>
@@ -695,11 +716,22 @@
       <c r="ALU8" s="8"/>
     </row>
     <row r="9" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>23</v>
+      </c>
       <c r="D9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="I9" s="11"/>
       <c r="ALS9" s="8"/>

</xml_diff>

<commit_message>
feat：update 3 light dragon
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
+++ b/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -97,13 +97,46 @@
     <t xml:space="preserve">-60|0|70</t>
   </si>
   <si>
-    <t xml:space="preserve">0|0|-25</t>
+    <t xml:space="preserve">0|0|0</t>
   </si>
   <si>
     <t xml:space="preserve">7769FA77488F5E75A8D3B19B260CB297</t>
   </si>
   <si>
     <t xml:space="preserve">-90|0|93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32DA891F44CC6CE6F3F09E91FB08D87C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5C036F804C66CAC8064CCAAC1DCF6F49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC7D76B94E521E9A022F869AD65192C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59CDB7A54052A7FB5BA4C3A3245415DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30|0|100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEBAD0B541B4F7294F82EC8D69634024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0|0|70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0992CA8B43AB93BB11354E8519E10987</t>
   </si>
 </sst>
 </file>
@@ -495,7 +528,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topRight" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -788,8 +821,73 @@
         <v>27</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="15" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
+      <c r="A15" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="G15" s="11"/>
       <c r="I15" s="11"/>
       <c r="ALS15" s="8"/>
@@ -797,10 +895,22 @@
       <c r="ALU15" s="8"/>
     </row>
     <row r="16" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="A16" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="13" t="n">
+        <v>23</v>
+      </c>
       <c r="D16" s="13"/>
+      <c r="E16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
       <c r="I16" s="11"/>
@@ -811,7 +921,21 @@
       <c r="ALU16" s="8"/>
     </row>
     <row r="17" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
+      <c r="A17" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="I17" s="11"/>
       <c r="ALS17" s="8"/>

</xml_diff>

<commit_message>
feat：update world1 stage excel and dark2
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
+++ b/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t xml:space="preserve">0|0|30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1C29B9D94B65461433D3B889663D9CD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2954B0C346525118F420E78A380529FA</t>
   </si>
 </sst>
 </file>
@@ -540,7 +546,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topRight" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1987,6 +1993,40 @@
         <v>42</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="24" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="7"/>
       <c r="I24" s="7"/>

</xml_diff>

<commit_message>
feat：update 2 drak dragon and nerReUI8
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
+++ b/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t xml:space="preserve">2954B0C346525118F420E78A380529FA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BF4E72324C697972203BCE924213B11A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AE095FD54159A3110B3CCAB3D6135FA3</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topRight" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2027,6 +2033,40 @@
         <v>25</v>
       </c>
     </row>
+    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="24" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="7"/>
       <c r="I24" s="7"/>

</xml_diff>

<commit_message>
feat：update dark dragon 5—7
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
+++ b/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t xml:space="preserve">AE095FD54159A3110B3CCAB3D6135FA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9681BE7840BF796D9C6BB9A825A9958A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E01DE10645ACDE36CF1B2B84113E18E6</t>
   </si>
 </sst>
 </file>
@@ -549,10 +555,10 @@
   </sheetPr>
   <dimension ref="A1:ALU376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="D4" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topRight" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2068,6 +2074,21 @@
       </c>
     </row>
     <row r="24" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="I24" s="7"/>
       <c r="ALS24" s="8"/>
@@ -2075,6 +2096,21 @@
       <c r="ALU24" s="8"/>
     </row>
     <row r="25" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="I25" s="7"/>
       <c r="ALS25" s="8"/>

</xml_diff>

<commit_message>
feat：update dodo level up
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
+++ b/nevergiveup/Excel/LevelEffect_升级特效表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -191,6 +191,36 @@
   </si>
   <si>
     <t xml:space="preserve">BC14680340D9DF99A552FE8BED2B6B1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D7CE4FAB4567042A4A6DEEA40BB3B3B9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4A1B1ED642AAC5CFE7E5A4AE28FC737D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5144EECC4DC875FAC47567B0EB760E16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2D94D5E4058E176BDD1AC983EE8BC4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB9CCAAE47B1F0618FE9148C40267692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6B88953408E5440C0B7BB930F1322A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8C3306E34575EBDD93302889729CBAEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8DB371804BF82BDD42A986B20237A2F8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69D63DB64AB5006F7A51C5B3738EE46A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7F1ADBE2438571300DA7268761EBEB2A</t>
   </si>
 </sst>
 </file>
@@ -579,10 +609,10 @@
   </sheetPr>
   <dimension ref="A1:ALU376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="E40" activeCellId="0" sqref="E40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="D22" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topRight" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2019,10 +2049,11 @@
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -2036,10 +2067,11 @@
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="6" t="s">
@@ -2053,10 +2085,11 @@
       <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -2070,10 +2103,11 @@
       <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="6" t="s">
@@ -2087,10 +2121,11 @@
       <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="n">
+      <c r="C23" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -2318,6 +2353,21 @@
       <c r="ALU33" s="8"/>
     </row>
     <row r="34" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G34" s="7"/>
       <c r="I34" s="7"/>
       <c r="ALS34" s="8"/>
@@ -2325,6 +2375,21 @@
       <c r="ALU34" s="8"/>
     </row>
     <row r="35" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E35" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G35" s="7"/>
       <c r="I35" s="7"/>
       <c r="ALS35" s="8"/>
@@ -2332,6 +2397,21 @@
       <c r="ALU35" s="8"/>
     </row>
     <row r="36" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E36" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G36" s="7"/>
       <c r="I36" s="7"/>
       <c r="ALS36" s="8"/>
@@ -2339,6 +2419,21 @@
       <c r="ALU36" s="8"/>
     </row>
     <row r="37" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E37" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="I37" s="7"/>
       <c r="ALS37" s="8"/>
@@ -2346,6 +2441,21 @@
       <c r="ALU37" s="8"/>
     </row>
     <row r="38" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G38" s="7"/>
       <c r="I38" s="7"/>
       <c r="ALS38" s="8"/>
@@ -2353,6 +2463,21 @@
       <c r="ALU38" s="8"/>
     </row>
     <row r="39" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E39" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G39" s="7"/>
       <c r="I39" s="7"/>
       <c r="ALS39" s="8"/>
@@ -2360,6 +2485,21 @@
       <c r="ALU39" s="8"/>
     </row>
     <row r="40" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E40" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G40" s="7"/>
       <c r="I40" s="7"/>
       <c r="ALS40" s="8"/>
@@ -2367,6 +2507,21 @@
       <c r="ALU40" s="8"/>
     </row>
     <row r="41" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E41" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G41" s="7"/>
       <c r="I41" s="7"/>
       <c r="ALS41" s="8"/>
@@ -2374,6 +2529,21 @@
       <c r="ALU41" s="8"/>
     </row>
     <row r="42" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E42" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G42" s="7"/>
       <c r="I42" s="7"/>
       <c r="ALS42" s="8"/>
@@ -2381,6 +2551,21 @@
       <c r="ALU42" s="8"/>
     </row>
     <row r="43" s="6" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E43" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G43" s="7"/>
       <c r="I43" s="7"/>
       <c r="ALS43" s="8"/>

</xml_diff>